<commit_message>
parte 1 - segunda revision
</commit_message>
<xml_diff>
--- a/tablas.xlsx
+++ b/tablas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\Estadistica-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indecok-my.sharepoint.com/personal/agomezvargas_indec_gob_ar/Documents/Documentos/GitHub/Estadistica 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213E5CCE-8C82-455F-9646-A79DEA0A399E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{213E5CCE-8C82-455F-9646-A79DEA0A399E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{351F0874-3A63-466D-9B06-4CA652B1A0D8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{61171B79-1E06-4B85-9DD1-708305727F37}"/>
+    <workbookView xWindow="24552" yWindow="-1728" windowWidth="17280" windowHeight="8964" xr2:uid="{61171B79-1E06-4B85-9DD1-708305727F37}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -63,17 +63,6 @@
     <t>temperaturas en grados Fahrenheit o Celsius</t>
   </si>
   <si>
-    <t>Estado civil
-Color de ojos</t>
-  </si>
-  <si>
-    <t>Nivel educativo</t>
-  </si>
-  <si>
-    <t>Altura
-Peso</t>
-  </si>
-  <si>
     <t>Las categorías están ordenadas, pero no hay diferencias o estas carecen de significado.</t>
   </si>
   <si>
@@ -307,6 +296,17 @@
   </si>
   <si>
     <t>libros</t>
+  </si>
+  <si>
+    <t>Estado civil | 
+Color de ojos</t>
+  </si>
+  <si>
+    <t>Nivel educativo | Grado militar</t>
+  </si>
+  <si>
+    <t>Altura | 
+Peso</t>
   </si>
 </sst>
 </file>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4ED38B2-53D4-4BA8-8C67-50B124050679}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -719,21 +719,21 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -741,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -752,10 +752,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -767,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA99093-A7DA-4A63-9627-3F634BCECA4C}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -780,22 +780,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
@@ -803,19 +803,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -823,19 +823,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -843,19 +843,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="216" x14ac:dyDescent="0.3">
@@ -863,19 +863,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="388.8" x14ac:dyDescent="0.3">
@@ -883,19 +883,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -903,19 +903,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -923,19 +923,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
@@ -943,19 +943,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -963,19 +963,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -983,19 +983,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
@@ -1003,19 +1003,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1023,19 +1023,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -1043,19 +1043,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
@@ -1063,19 +1063,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1083,19 +1083,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1103,19 +1103,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correciones 1 y 2, sumo 3 y 4 faltantes
</commit_message>
<xml_diff>
--- a/tablas.xlsx
+++ b/tablas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indecok-my.sharepoint.com/personal/agomezvargas_indec_gob_ar/Documents/Documentos/GitHub/Estadistica 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\Estadistica-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{213E5CCE-8C82-455F-9646-A79DEA0A399E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{351F0874-3A63-466D-9B06-4CA652B1A0D8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E350ABC-F6EC-4DED-834E-E290F271C9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24552" yWindow="-1728" windowWidth="17280" windowHeight="8964" xr2:uid="{61171B79-1E06-4B85-9DD1-708305727F37}"/>
+    <workbookView xWindow="0" yWindow="732" windowWidth="21600" windowHeight="11232" activeTab="1" xr2:uid="{61171B79-1E06-4B85-9DD1-708305727F37}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -165,124 +165,133 @@
     <t>NOMINAL</t>
   </si>
   <si>
-    <t>Beber, ir de copas, bailar (1)
+    <t>DE INTÉRVALO</t>
+  </si>
+  <si>
+    <t>HORAS</t>
+  </si>
+  <si>
+    <t>ORDINAL</t>
+  </si>
+  <si>
+    <t>Grado de dedicación en las tareas del hogar</t>
+  </si>
+  <si>
+    <t>grado de felicidad en la infancia</t>
+  </si>
+  <si>
+    <t>horas libres semanales para ocio</t>
+  </si>
+  <si>
+    <t>horas semanales dedicadas a ver tv</t>
+  </si>
+  <si>
+    <t>INTÉRVALO</t>
+  </si>
+  <si>
+    <t>cantidad de hijos que creé va a tener</t>
+  </si>
+  <si>
+    <t>cantidad de hijos que le gustaría llegar a tener</t>
+  </si>
+  <si>
+    <t>lugar de estudios</t>
+  </si>
+  <si>
+    <t>cantidad de libros leidos en 12 meses</t>
+  </si>
+  <si>
+    <t>inclinación política</t>
+  </si>
+  <si>
+    <t>situación vincular/afectiva</t>
+  </si>
+  <si>
+    <t>autodefinición religiosa</t>
+  </si>
+  <si>
+    <t>grado de inclinación política de 1 a 10, siendo 1 más inclinado hacia la izquierda y 10 más inclinado a la derecha</t>
+  </si>
+  <si>
+    <t>rango de ingresos mensual de todos los miembros del hogar</t>
+  </si>
+  <si>
+    <t>rango de ingreso mensual por tipo de ingreso</t>
+  </si>
+  <si>
+    <t>sexo</t>
+  </si>
+  <si>
+    <t>edad</t>
+  </si>
+  <si>
+    <t>libros</t>
+  </si>
+  <si>
+    <t>Estado civil | 
+Color de ojos</t>
+  </si>
+  <si>
+    <t>Nivel educativo | Grado militar</t>
+  </si>
+  <si>
+    <t>Altura | 
+Peso</t>
+  </si>
+  <si>
+    <t>0,1,2,3,4,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- La etapa más feliz de tu vida 1
+- Una etapa más feliz que otras 2
+- Una etapa igual de feliz que otras 3
+- Una etapa menos feliz que otras 4
+- La etapa menos feliz de tu vida 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- Beber, ir de copas, bailar (1)
 - Hacer deportes (2)
--Viajes, excursiones (3)
+- Viajes, excursiones (3)
 - Ir al cine, al teatro (4)
 - Ir a museos, ir a conciertos (5)
 - Leer (6)
 - Otra (7)</t>
   </si>
   <si>
-    <t>DE INTÉRVALO</t>
-  </si>
-  <si>
-    <t>HORAS</t>
-  </si>
-  <si>
-    <t>La etapa más feliz de tu vida 1
-- Una etapa más feliz que otras 2
-- Una etapa igual de feliz que otras 3
-- Una etapa menos feliz que otras 4
-- La etapa menos feliz de tu vida 5</t>
-  </si>
-  <si>
-    <t>ORDINAL</t>
-  </si>
-  <si>
-    <t>Grado de dedicación en las tareas del hogar</t>
-  </si>
-  <si>
-    <t>grado de felicidad en la infancia</t>
-  </si>
-  <si>
-    <t>tareas del hogar: Hacer la cama, Limpiar la casa, Cuidar de los hijos o hermanos pequeños
-&lt;br&gt;
-grado de dedicación; 
-1. No suelo hacerlo nunca
-2. Solo lo hago en ocasiones
-3. Comparto esta tarea con otra/s personas
-4. Recae en mi toda la responsabilidad y suelo hacerlo siempre</t>
-  </si>
-  <si>
-    <t>horas libres semanales para ocio</t>
-  </si>
-  <si>
-    <t>horas semanales dedicadas a ver tv</t>
-  </si>
-  <si>
-    <t>INTÉRVALO</t>
-  </si>
-  <si>
-    <t>0 a 5</t>
-  </si>
-  <si>
-    <t>cantidad de hijos que creé va a tener</t>
-  </si>
-  <si>
-    <t>cantidad de hijos que le gustaría llegar a tener</t>
-  </si>
-  <si>
-    <t>Tienes novio/a formal 1
--Ahora no tienes novio/a formal 2
--Hasta ahora solo has tenido relaciones afectivas pasajeras 3
--Nunca has tenido una relación especial con un chico/a 4</t>
-  </si>
-  <si>
-    <t>lugar de estudios</t>
-  </si>
-  <si>
-    <t>En un centro estatal, público
--En un centro privado, no religioso
--En un centro privado, religioso</t>
-  </si>
-  <si>
-    <t>cantidad de libros leidos en 12 meses</t>
-  </si>
-  <si>
-    <t>Católico practicante 1
+    <t xml:space="preserve">
+- Tienes novio/a formal 1
+- Ahora no tienes novio/a formal 2
+- Hasta ahora solo has tenido relaciones afectivas pasajeras 3
+- Nunca has tenido una relación especial con un chico/a 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- En un centro estatal, público
+- En un centro privado, no religioso
+- En un centro privado, religioso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- Católico practicante 1
 - Católico no practicante 2
 - Creyente de otra religión 3
 - No creyente 4
 - Indiferente 5</t>
   </si>
   <si>
-    <t>inclinación política</t>
-  </si>
-  <si>
-    <t>situación vincular/afectiva</t>
-  </si>
-  <si>
-    <t>autodefinición religiosa</t>
-  </si>
-  <si>
-    <t>grado de inclinación política de 1 a 10, siendo 1 más inclinado hacia la izquierda y 10 más inclinado a la derecha</t>
-  </si>
-  <si>
-    <t>Ingresos personales
+    <t xml:space="preserve">
+- Ingresos personales
 - Ingresos de tu pareja 
 - Aportaciones familiares
 - Otros</t>
   </si>
   <si>
-    <t>rango de ingresos mensual de todos los miembros del hogar</t>
-  </si>
-  <si>
-    <t>rango de ingreso mensual por tipo de ingreso</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hombre (1)
-- Mujer (2)</t>
-  </si>
-  <si>
-    <t>sexo</t>
-  </si>
-  <si>
-    <t>edad</t>
-  </si>
-  <si>
-    <t>Menos o igual a 50.000 pts (01)
-- De 50.000 a 100.000 pts (02)  - De 100.001 a 150.000 pts (03)
+    <t xml:space="preserve">
+- Menos o igual a 50.000 pts (01)
+- De 50.000 a 100.000 pts (02)  
+- De 100.001 a 150.000 pts (03)
 - De 150.001 a 200.000 pts (04)
 - De 200.001 a 300.000 pts (05)
 - De 300.001 a 400.000 pts (06)
@@ -292,21 +301,23 @@
 - Más de 1 millón de pts (10)</t>
   </si>
   <si>
-    <t xml:space="preserve">rangos etário de 17 a 29 </t>
-  </si>
-  <si>
-    <t>libros</t>
-  </si>
-  <si>
-    <t>Estado civil | 
-Color de ojos</t>
-  </si>
-  <si>
-    <t>Nivel educativo | Grado militar</t>
-  </si>
-  <si>
-    <t>Altura | 
-Peso</t>
+    <t xml:space="preserve">
+- Hombre (1)
+- Mujer (2)</t>
+  </si>
+  <si>
+    <t>17,18,... 29</t>
+  </si>
+  <si>
+    <t>_tareas del hogar_: 
+- Hacer la cama
+- Limpiar la casa
+- Cuidar de los hijos o hermanos pequeños. &lt;br&gt; &lt;br&gt;
+_grado de dedicación_: 
+1. No suelo hacerlo nunca
+2. Solo lo hago en ocasiones
+3. Comparto esta tarea con otra/s personas
+4. Recae en mi toda la responsabilidad y suelo hacerlo siempre</t>
   </si>
 </sst>
 </file>
@@ -692,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4ED38B2-53D4-4BA8-8C67-50B124050679}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,7 +733,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -733,7 +744,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -755,7 +766,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -767,15 +778,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA99093-A7DA-4A63-9627-3F634BCECA4C}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" style="3"/>
     <col min="2" max="2" width="11.5546875" style="2"/>
-    <col min="3" max="6" width="11.5546875" style="3"/>
+    <col min="3" max="4" width="11.5546875" style="3"/>
+    <col min="5" max="5" width="22" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -798,7 +811,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -812,7 +825,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>41</v>
@@ -829,13 +842,13 @@
         <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -849,16 +862,16 @@
         <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -869,16 +882,16 @@
         <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="388.8" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -889,13 +902,13 @@
         <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -909,13 +922,13 @@
         <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -929,16 +942,16 @@
         <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -949,16 +962,16 @@
         <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -969,10 +982,10 @@
         <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>41</v>
@@ -989,16 +1002,16 @@
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1009,10 +1022,10 @@
         <v>28</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>41</v>
@@ -1029,16 +1042,16 @@
         <v>29</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1049,16 +1062,16 @@
         <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1069,16 +1082,16 @@
         <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1089,10 +1102,10 @@
         <v>32</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>41</v>
@@ -1109,13 +1122,13 @@
         <v>33</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>